<commit_message>
this is modified myexcel repositery
</commit_message>
<xml_diff>
--- a/myexcel.xlsx
+++ b/myexcel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ankit\OneDrive\Desktop\git tutorial\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E775B52-3466-4201-B1CD-CC450B8B5FA8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D1293BC-10FA-49FD-9524-FD10B78D1CEC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>kajhf</t>
   </si>
@@ -33,7 +33,13 @@
     <t>kdhfa</t>
   </si>
   <si>
-    <t>SHEF</t>
+    <t>sfawfh</t>
+  </si>
+  <si>
+    <t>oAHSFIyfe</t>
+  </si>
+  <si>
+    <t>iuhefiuHWEF;</t>
   </si>
 </sst>
 </file>
@@ -351,27 +357,37 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I13"/>
+  <dimension ref="A1:M16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="H11" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="M12" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="I13" t="s">
         <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="K16" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>